<commit_message>
Suite Allure Report+Negotiation with DB
</commit_message>
<xml_diff>
--- a/src/test/resources/Documents/1076/Actual/JobMaterial.xlsx
+++ b/src/test/resources/Documents/1076/Actual/JobMaterial.xlsx
@@ -65,46 +65,46 @@
     <t/>
   </si>
   <si>
+    <t xml:space="preserve">Black - UV - </t>
+  </si>
+  <si>
+    <t>10001817 - 9409 MIXING BLACK UV - INK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyan - UV - </t>
+  </si>
+  <si>
+    <t>10001837 - 9443 PRO CYAN BW8 UV - INK</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yellow - UV - </t>
   </si>
   <si>
     <t>10001305 - PROCESS YELLOW C UV</t>
   </si>
   <si>
-    <t xml:space="preserve">Black - UV - </t>
-  </si>
-  <si>
-    <t>10001817 - 9409 MIXING BLACK UV - INK</t>
-  </si>
-  <si>
     <t xml:space="preserve">Magenta - UV - </t>
   </si>
   <si>
     <t>10001836 - 9442 PRO MAGENTA BW5 UV - INK</t>
   </si>
   <si>
-    <t xml:space="preserve">Cyan - UV - </t>
-  </si>
-  <si>
-    <t>10001837 - 9443 PRO CYAN BW8 UV - INK</t>
-  </si>
-  <si>
     <t>Glue 0x0 (Varnish 1x1)</t>
   </si>
   <si>
+    <t>Adhesive</t>
+  </si>
+  <si>
+    <t>0.22</t>
+  </si>
+  <si>
+    <t>10001053 - RAVENWOOD LINERLESS-ADHESIVE - 7445HD</t>
+  </si>
+  <si>
     <t>Silicone</t>
   </si>
   <si>
-    <t>0.22</t>
-  </si>
-  <si>
     <t>10016451 - Evonik RW 10 Teco RC Silicone</t>
-  </si>
-  <si>
-    <t>Adhesive</t>
-  </si>
-  <si>
-    <t>10001053 - RAVENWOOD LINERLESS-ADHESIVE - 7445HD</t>
   </si>
   <si>
     <t>Roll</t>

</xml_diff>

<commit_message>
Not sure, may be edited part
</commit_message>
<xml_diff>
--- a/src/test/resources/Documents/1076/Actual/JobMaterial.xlsx
+++ b/src/test/resources/Documents/1076/Actual/JobMaterial.xlsx
@@ -53,16 +53,28 @@
     <t>Flexo press 5x0</t>
   </si>
   <si>
+    <t xml:space="preserve">Magenta - UV - </t>
+  </si>
+  <si>
+    <t>0.29</t>
+  </si>
+  <si>
+    <t>lbs</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>10001836 - 9442 PRO MAGENTA BW5 UV - INK</t>
+  </si>
+  <si>
     <t xml:space="preserve">PANTONE Yellow U  - UV - </t>
   </si>
   <si>
-    <t>0.29</t>
-  </si>
-  <si>
-    <t>lbs</t>
-  </si>
-  <si>
-    <t/>
+    <t xml:space="preserve">Cyan - UV - </t>
+  </si>
+  <si>
+    <t>10001837 - 9443 PRO CYAN BW8 UV - INK</t>
   </si>
   <si>
     <t xml:space="preserve">Black - UV - </t>
@@ -71,40 +83,28 @@
     <t>10001817 - 9409 MIXING BLACK UV - INK</t>
   </si>
   <si>
-    <t xml:space="preserve">Cyan - UV - </t>
-  </si>
-  <si>
-    <t>10001837 - 9443 PRO CYAN BW8 UV - INK</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yellow - UV - </t>
   </si>
   <si>
     <t>10001305 - PROCESS YELLOW C UV</t>
   </si>
   <si>
-    <t xml:space="preserve">Magenta - UV - </t>
-  </si>
-  <si>
-    <t>10001836 - 9442 PRO MAGENTA BW5 UV - INK</t>
-  </si>
-  <si>
     <t>Glue 0x0 (Varnish 1x1)</t>
   </si>
   <si>
+    <t>Silicone</t>
+  </si>
+  <si>
+    <t>0.22</t>
+  </si>
+  <si>
+    <t>10016451 - Evonik RW 10 Teco RC Silicone</t>
+  </si>
+  <si>
     <t>Adhesive</t>
   </si>
   <si>
-    <t>0.22</t>
-  </si>
-  <si>
     <t>10001053 - RAVENWOOD LINERLESS-ADHESIVE - 7445HD</t>
-  </si>
-  <si>
-    <t>Silicone</t>
-  </si>
-  <si>
-    <t>10016451 - Evonik RW 10 Teco RC Silicone</t>
   </si>
   <si>
     <t>Roll</t>
@@ -612,7 +612,7 @@
         <v>16</v>
       </c>
       <c r="H2" t="s" s="9">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -626,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s" s="13">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s" s="14">
         <v>14</v>
@@ -638,7 +638,7 @@
         <v>16</v>
       </c>
       <c r="H3" t="s" s="17">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">

</xml_diff>